<commit_message>
Working loading of library
</commit_message>
<xml_diff>
--- a/VareTypeBibliotek.xlsx
+++ b/VareTypeBibliotek.xlsx
@@ -3286,23 +3286,7 @@
     <t xml:space="preserve">Minimælk Arla</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Arla </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Minimælk</t>
-    </r>
+    <t xml:space="preserve">Arla Minimælk</t>
   </si>
   <si>
     <t xml:space="preserve">Naturli Pølse</t>
@@ -5988,7 +5972,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -6024,11 +6008,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -6108,7 +6087,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6297,8 +6276,8 @@
   </sheetPr>
   <dimension ref="A1:C1793"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A896" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C904" activeCellId="0" sqref="C904"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>